<commit_message>
Fixed issues with JST PH header orientation.
</commit_message>
<xml_diff>
--- a/production/v0p1_r1/CPL_JLCPCB_feather_tripler_enc1_v0p1r1.xlsx
+++ b/production/v0p1_r1/CPL_JLCPCB_feather_tripler_enc1_v0p1r1.xlsx
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -100,6 +100,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -159,7 +166,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,6 +180,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,7 +207,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,17 +243,17 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>146.812</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="B2" s="4" t="n">
+        <v>147.212</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>-64.2874</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -251,17 +262,17 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>146.812</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="4" t="n">
+        <v>147.212</v>
+      </c>
+      <c r="C3" s="4" t="n">
         <v>-80.7974</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -270,17 +281,17 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>146.812</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4" s="4" t="n">
+        <v>147.212</v>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>-97.3074</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -342,6 +353,12 @@
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
     </row>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>